<commit_message>
extracted heuristic data for pdfplumber and spacy data
</commit_message>
<xml_diff>
--- a/ExtractedData/HeuristicData/output_Adidas.xlsx
+++ b/ExtractedData/HeuristicData/output_Adidas.xlsx
@@ -14,15 +14,18 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>Processing</t>
   </si>
   <si>
-    <t>AI</t>
-  </si>
-  <si>
-    <t>Technology</t>
+    <t>AI-Synonyms</t>
+  </si>
+  <si>
+    <t>Product-AI</t>
+  </si>
+  <si>
+    <t>Business-Process-AI</t>
   </si>
   <si>
     <t>Data</t>
@@ -419,13 +422,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F12"/>
+  <dimension ref="A1:G12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:7">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -441,225 +444,261 @@
       <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:6">
+      <c r="G1" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
       <c r="A2" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B2">
-        <v>0</v>
+        <v>53</v>
       </c>
       <c r="C2">
-        <v>546</v>
+        <v>9</v>
       </c>
       <c r="D2">
-        <v>191</v>
+        <v>1</v>
       </c>
       <c r="E2">
         <v>0</v>
       </c>
       <c r="F2">
+        <v>3</v>
+      </c>
+      <c r="G2">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
+      <c r="A3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3">
+        <v>62</v>
+      </c>
+      <c r="C3">
+        <v>10</v>
+      </c>
+      <c r="D3">
+        <v>2</v>
+      </c>
+      <c r="E3">
+        <v>0</v>
+      </c>
+      <c r="F3">
+        <v>10</v>
+      </c>
+      <c r="G3">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
+      <c r="A4" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4">
+        <v>56</v>
+      </c>
+      <c r="C4">
+        <v>8</v>
+      </c>
+      <c r="D4">
+        <v>3</v>
+      </c>
+      <c r="E4">
+        <v>0</v>
+      </c>
+      <c r="F4">
+        <v>12</v>
+      </c>
+      <c r="G4">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
+      <c r="A5" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5">
+        <v>59</v>
+      </c>
+      <c r="C5">
+        <v>3</v>
+      </c>
+      <c r="D5">
+        <v>2</v>
+      </c>
+      <c r="E5">
+        <v>1</v>
+      </c>
+      <c r="F5">
+        <v>11</v>
+      </c>
+      <c r="G5">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7">
+      <c r="A6" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6">
+        <v>64</v>
+      </c>
+      <c r="C6">
+        <v>4</v>
+      </c>
+      <c r="D6">
+        <v>3</v>
+      </c>
+      <c r="E6">
+        <v>0</v>
+      </c>
+      <c r="F6">
+        <v>10</v>
+      </c>
+      <c r="G6">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7">
+      <c r="A7" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7">
+        <v>74</v>
+      </c>
+      <c r="C7">
         <v>6</v>
       </c>
-    </row>
-    <row r="3" spans="1:6">
-      <c r="A3" s="1" t="s">
+      <c r="D7">
+        <v>1</v>
+      </c>
+      <c r="E7">
+        <v>0</v>
+      </c>
+      <c r="F7">
+        <v>15</v>
+      </c>
+      <c r="G7">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7">
+      <c r="A8" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B8">
+        <v>66</v>
+      </c>
+      <c r="C8">
+        <v>12</v>
+      </c>
+      <c r="D8">
+        <v>1</v>
+      </c>
+      <c r="E8">
+        <v>0</v>
+      </c>
+      <c r="F8">
+        <v>15</v>
+      </c>
+      <c r="G8">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7">
+      <c r="A9" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B9">
+        <v>96</v>
+      </c>
+      <c r="C9">
+        <v>19</v>
+      </c>
+      <c r="D9">
+        <v>11</v>
+      </c>
+      <c r="E9">
+        <v>0</v>
+      </c>
+      <c r="F9">
+        <v>35</v>
+      </c>
+      <c r="G9">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7">
+      <c r="A10" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B10">
+        <v>99</v>
+      </c>
+      <c r="C10">
+        <v>20</v>
+      </c>
+      <c r="D10">
+        <v>4</v>
+      </c>
+      <c r="E10">
+        <v>0</v>
+      </c>
+      <c r="F10">
+        <v>37</v>
+      </c>
+      <c r="G10">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7">
+      <c r="A11" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B11">
+        <v>87</v>
+      </c>
+      <c r="C11">
+        <v>12</v>
+      </c>
+      <c r="D11">
+        <v>7</v>
+      </c>
+      <c r="E11">
+        <v>1</v>
+      </c>
+      <c r="F11">
+        <v>39</v>
+      </c>
+      <c r="G11">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7">
+      <c r="A12" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B12">
+        <v>87</v>
+      </c>
+      <c r="C12">
         <v>6</v>
       </c>
-      <c r="B3">
-        <v>0</v>
-      </c>
-      <c r="C3">
-        <v>0</v>
-      </c>
-      <c r="D3">
-        <v>0</v>
-      </c>
-      <c r="E3">
-        <v>0</v>
-      </c>
-      <c r="F3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6">
-      <c r="A4" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B4">
-        <v>0</v>
-      </c>
-      <c r="C4">
-        <v>628</v>
-      </c>
-      <c r="D4">
-        <v>228</v>
-      </c>
-      <c r="E4">
-        <v>1</v>
-      </c>
-      <c r="F4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6">
-      <c r="A5" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B5">
-        <v>0</v>
-      </c>
-      <c r="C5">
-        <v>527</v>
-      </c>
-      <c r="D5">
-        <v>170</v>
-      </c>
-      <c r="E5">
+      <c r="D12">
         <v>2</v>
       </c>
-      <c r="F5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6">
-      <c r="A6" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B6">
-        <v>0</v>
-      </c>
-      <c r="C6">
-        <v>383</v>
-      </c>
-      <c r="D6">
-        <v>134</v>
-      </c>
-      <c r="E6">
-        <v>3</v>
-      </c>
-      <c r="F6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6">
-      <c r="A7" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B7">
-        <v>0</v>
-      </c>
-      <c r="C7">
-        <v>406</v>
-      </c>
-      <c r="D7">
-        <v>113</v>
-      </c>
-      <c r="E7">
-        <v>5</v>
-      </c>
-      <c r="F7">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6">
-      <c r="A8" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B8">
-        <v>0</v>
-      </c>
-      <c r="C8">
-        <v>409</v>
-      </c>
-      <c r="D8">
-        <v>105</v>
-      </c>
-      <c r="E8">
-        <v>3</v>
-      </c>
-      <c r="F8">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6">
-      <c r="A9" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B9">
-        <v>0</v>
-      </c>
-      <c r="C9">
-        <v>501</v>
-      </c>
-      <c r="D9">
-        <v>101</v>
-      </c>
-      <c r="E9">
-        <v>4</v>
-      </c>
-      <c r="F9">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6">
-      <c r="A10" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B10">
-        <v>0</v>
-      </c>
-      <c r="C10">
-        <v>509</v>
-      </c>
-      <c r="D10">
-        <v>109</v>
-      </c>
-      <c r="E10">
-        <v>11</v>
-      </c>
-      <c r="F10">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6">
-      <c r="A11" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B11">
-        <v>0</v>
-      </c>
-      <c r="C11">
-        <v>430</v>
-      </c>
-      <c r="D11">
-        <v>103</v>
-      </c>
-      <c r="E11">
-        <v>8</v>
-      </c>
-      <c r="F11">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6">
-      <c r="A12" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B12">
-        <v>0</v>
-      </c>
-      <c r="C12">
-        <v>342</v>
-      </c>
-      <c r="D12">
-        <v>96</v>
-      </c>
       <c r="E12">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="F12">
-        <v>0</v>
+        <v>46</v>
+      </c>
+      <c r="G12">
+        <v>52</v>
       </c>
     </row>
   </sheetData>

</xml_diff>